<commit_message>
updating Auxilirary Parts Stats
</commit_message>
<xml_diff>
--- a/Data/Weapons.xlsx
+++ b/Data/Weapons.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="679">
   <si>
     <t>Name</t>
   </si>
@@ -421,6 +421,9 @@
     <t>Bushmaster ACR</t>
   </si>
   <si>
+    <t>CMMG Mk47 Mutant</t>
+  </si>
+  <si>
     <t>CZ Bren 2 / CZ BREN 805</t>
   </si>
   <si>
@@ -454,9 +457,6 @@
     <t>Knight's Armament Company PDW</t>
   </si>
   <si>
-    <t>KS-47 MK-47</t>
-  </si>
-  <si>
     <t>KSVK 12.7</t>
   </si>
   <si>
@@ -494,6 +494,9 @@
   </si>
   <si>
     <t>PP-19 Bizon</t>
+  </si>
+  <si>
+    <t>Rifle Dynamics 704 Pistol</t>
   </si>
   <si>
     <t>RPD</t>
@@ -953,6 +956,9 @@
     <t>Confirmed on Reddit</t>
   </si>
   <si>
+    <t>Facebook, Twitter 1, Twitter 2</t>
+  </si>
+  <si>
     <t>Confirmed on russian audiopodcast with BSG</t>
   </si>
   <si>
@@ -972,9 +978,6 @@
     <t>Several sounds are present in the game files. These sounds are identical to the KAC PDW in Contract Wars. (Confirmed in Instagram photo)</t>
   </si>
   <si>
-    <t>Facebook</t>
-  </si>
-  <si>
     <t>Revealed in TarkovTV LIVE on 26.3.2021</t>
   </si>
   <si>
@@ -991,6 +994,9 @@
   </si>
   <si>
     <t>Confirmed, but not revealed</t>
+  </si>
+  <si>
+    <t>https://twitter.com/bstategames/status/1390304853033816069?s=20</t>
   </si>
   <si>
     <t>Confirmed on Reddit and an Instagram video</t>
@@ -1887,6 +1893,9 @@
     <t>https://static.wikia.nocookie.net/escapefromtarkov_gamepedia/images/5/53/Upcoming_acr.jpg/revision/latest/scale-to-width-down/180?cb=20180306161407</t>
   </si>
   <si>
+    <t>https://static.wikia.nocookie.net/escapefromtarkov_gamepedia/images/3/33/Mutant_Preview.jpg/revision/latest/scale-to-width-down/180?cb=20210507231557</t>
+  </si>
+  <si>
     <t>https://static.wikia.nocookie.net/escapefromtarkov_gamepedia/images/8/8b/CZ_BREN_2.jpg/revision/latest/scale-to-width-down/180?cb=20190213181027</t>
   </si>
   <si>
@@ -1920,9 +1929,6 @@
     <t>https://static.wikia.nocookie.net/escapefromtarkov_gamepedia/images/b/b4/KnightsArmamentCompany-PDW.gif/revision/latest/scale-to-width-down/180?cb=20190221155447</t>
   </si>
   <si>
-    <t>https://static.wikia.nocookie.net/escapefromtarkov_gamepedia/images/b/b1/KS-47_MK47.jpg/revision/latest/scale-to-width-down/180?cb=20210315204227</t>
-  </si>
-  <si>
     <t>https://static.wikia.nocookie.net/escapefromtarkov_gamepedia/images/5/59/KSVK_12.7.jpg/revision/latest/scale-to-width-down/180?cb=20190117142611</t>
   </si>
   <si>
@@ -1962,6 +1968,9 @@
     <t>https://static.wikia.nocookie.net/escapefromtarkov_gamepedia/images/6/6f/CW_Bizon.jpg/revision/latest/scale-to-width-down/180?cb=20190307235542</t>
   </si>
   <si>
+    <t>https://static.wikia.nocookie.net/escapefromtarkov_gamepedia/images/c/c7/RD704.jpg/revision/latest/scale-to-width-down/180?cb=20210508124419</t>
+  </si>
+  <si>
     <t>https://static.wikia.nocookie.net/escapefromtarkov_gamepedia/images/2/22/UPC_RPD.jpg/revision/latest/scale-to-width-down/180?cb=20190415164917</t>
   </si>
   <si>
@@ -1983,7 +1992,7 @@
     <t>https://static.wikia.nocookie.net/escapefromtarkov_gamepedia/images/c/cb/SR-3MP.jpg/revision/latest/scale-to-width-down/180?cb=20190117141145</t>
   </si>
   <si>
-    <t>https://static.wikia.nocookie.net/escapefromtarkov_gamepedia/images/4/42/Aug_.jpg/revision/latest/scale-to-width-down/300?cb=20201020141618</t>
+    <t>https://static.wikia.nocookie.net/escapefromtarkov_gamepedia/images/4/42/Aug_.jpg/revision/latest/scale-to-width-down/180?cb=20201020141618</t>
   </si>
   <si>
     <t>https://static.wikia.nocookie.net/escapefromtarkov_gamepedia/images/a/a2/SV-18.jpg/revision/latest/scale-to-width-down/180?cb=20190629082035</t>
@@ -2417,7 +2426,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I218"/>
+  <dimension ref="A1:I219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2457,19 +2466,19 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E2" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="F2" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2480,19 +2489,19 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D3" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E3" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="F3" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -2503,19 +2512,19 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D4" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E4" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="F4" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -2526,19 +2535,19 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D5" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E5" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="F5" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -2549,19 +2558,19 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D6" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E6" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="F6" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -2572,19 +2581,19 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D7" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E7" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="F7" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -2595,19 +2604,19 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D8" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E8" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="F8" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -2618,19 +2627,19 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D9" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E9" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="F9" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -2641,19 +2650,19 @@
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D10" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E10" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="F10" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -2664,19 +2673,19 @@
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D11" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E11" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="F11" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -2687,19 +2696,19 @@
         <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D12" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E12" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="F12" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -2710,19 +2719,19 @@
         <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D13" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E13" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="F13" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -2733,19 +2742,19 @@
         <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D14" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E14" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="F14" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -2756,19 +2765,19 @@
         <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D15" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E15" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="F15" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -2779,19 +2788,19 @@
         <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D16" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E16" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="F16" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -2802,19 +2811,19 @@
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D17" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E17" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="F17" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -2825,19 +2834,19 @@
         <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D18" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E18" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="F18" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -2848,19 +2857,19 @@
         <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D19" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E19" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="F19" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -2871,19 +2880,19 @@
         <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D20" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E20" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="F20" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -2894,19 +2903,19 @@
         <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D21" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E21" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F21" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -2917,19 +2926,19 @@
         <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D22" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E22" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="F22" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -2940,19 +2949,19 @@
         <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D23" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E23" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="F23" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -2963,19 +2972,19 @@
         <v>30</v>
       </c>
       <c r="C24" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D24" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E24" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="F24" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -2986,19 +2995,19 @@
         <v>31</v>
       </c>
       <c r="C25" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D25" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E25" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F25" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -3009,19 +3018,19 @@
         <v>32</v>
       </c>
       <c r="C26" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D26" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E26" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="F26" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -3032,19 +3041,19 @@
         <v>33</v>
       </c>
       <c r="C27" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D27" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E27" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="F27" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -3055,19 +3064,19 @@
         <v>34</v>
       </c>
       <c r="C28" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D28" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E28" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F28" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -3078,19 +3087,19 @@
         <v>35</v>
       </c>
       <c r="C29" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D29" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E29" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="F29" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -3101,19 +3110,19 @@
         <v>36</v>
       </c>
       <c r="C30" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D30" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E30" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="F30" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -3124,19 +3133,19 @@
         <v>37</v>
       </c>
       <c r="C31" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D31" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E31" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="F31" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -3153,10 +3162,10 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="F32" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="G32" t="s">
         <v>4</v>
@@ -3170,19 +3179,19 @@
         <v>38</v>
       </c>
       <c r="C33" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D33" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E33" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="F33" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -3193,19 +3202,19 @@
         <v>39</v>
       </c>
       <c r="C34" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D34" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E34" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="F34" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -3216,19 +3225,19 @@
         <v>40</v>
       </c>
       <c r="C35" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D35" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E35" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="F35" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -3245,10 +3254,10 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="F36" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="G36" t="s">
         <v>4</v>
@@ -3262,19 +3271,19 @@
         <v>41</v>
       </c>
       <c r="C37" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D37" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E37" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="F37" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -3291,10 +3300,10 @@
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="F38" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="G38" t="s">
         <v>4</v>
@@ -3308,19 +3317,19 @@
         <v>42</v>
       </c>
       <c r="C39" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D39" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E39" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="F39" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -3331,19 +3340,19 @@
         <v>43</v>
       </c>
       <c r="C40" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D40" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E40" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F40" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -3354,19 +3363,19 @@
         <v>44</v>
       </c>
       <c r="C41" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D41" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E41" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="F41" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -3377,19 +3386,19 @@
         <v>45</v>
       </c>
       <c r="C42" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D42" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E42" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="F42" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -3400,19 +3409,19 @@
         <v>46</v>
       </c>
       <c r="C43" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D43" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E43" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F43" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -3423,19 +3432,19 @@
         <v>47</v>
       </c>
       <c r="C44" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D44" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E44" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="F44" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -3446,19 +3455,19 @@
         <v>48</v>
       </c>
       <c r="C45" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D45" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E45" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="F45" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -3469,19 +3478,19 @@
         <v>49</v>
       </c>
       <c r="C46" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D46" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E46" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F46" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -3492,19 +3501,19 @@
         <v>50</v>
       </c>
       <c r="C47" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D47" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E47" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F47" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -3515,19 +3524,19 @@
         <v>51</v>
       </c>
       <c r="C48" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D48" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E48" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="F48" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -3538,19 +3547,19 @@
         <v>52</v>
       </c>
       <c r="C49" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D49" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E49" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F49" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -3561,19 +3570,19 @@
         <v>53</v>
       </c>
       <c r="C50" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D50" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E50" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F50" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -3584,19 +3593,19 @@
         <v>54</v>
       </c>
       <c r="C51" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D51" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E51" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="F51" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -3607,19 +3616,19 @@
         <v>55</v>
       </c>
       <c r="C52" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D52" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E52" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="F52" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -3630,19 +3639,19 @@
         <v>56</v>
       </c>
       <c r="C53" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D53" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E53" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="F53" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -3653,19 +3662,19 @@
         <v>57</v>
       </c>
       <c r="C54" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D54" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E54" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="F54" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -3676,19 +3685,19 @@
         <v>58</v>
       </c>
       <c r="C55" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D55" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E55" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="F55" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -3699,19 +3708,19 @@
         <v>59</v>
       </c>
       <c r="C56" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D56" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E56" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="F56" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -3728,10 +3737,10 @@
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="F57" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="G57" t="s">
         <v>4</v>
@@ -3745,19 +3754,19 @@
         <v>60</v>
       </c>
       <c r="C58" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D58" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E58" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F58" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -3768,19 +3777,19 @@
         <v>61</v>
       </c>
       <c r="C59" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D59" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E59" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F59" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -3791,19 +3800,19 @@
         <v>62</v>
       </c>
       <c r="C60" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D60" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E60" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F60" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -3814,19 +3823,19 @@
         <v>63</v>
       </c>
       <c r="C61" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D61" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E61" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="F61" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -3837,19 +3846,19 @@
         <v>64</v>
       </c>
       <c r="C62" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D62" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E62" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="F62" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -3860,19 +3869,19 @@
         <v>65</v>
       </c>
       <c r="C63" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D63" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E63" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F63" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -3883,19 +3892,19 @@
         <v>66</v>
       </c>
       <c r="C64" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D64" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E64" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F64" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -3912,10 +3921,10 @@
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="F65" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="G65" t="s">
         <v>4</v>
@@ -3929,19 +3938,19 @@
         <v>67</v>
       </c>
       <c r="C66" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D66" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E66" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F66" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -3952,19 +3961,19 @@
         <v>68</v>
       </c>
       <c r="C67" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D67" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E67" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F67" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -3975,19 +3984,19 @@
         <v>69</v>
       </c>
       <c r="C68" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D68" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E68" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F68" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -3998,19 +4007,19 @@
         <v>70</v>
       </c>
       <c r="C69" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D69" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E69" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F69" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -4021,19 +4030,19 @@
         <v>71</v>
       </c>
       <c r="C70" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D70" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E70" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F70" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -4044,19 +4053,19 @@
         <v>72</v>
       </c>
       <c r="C71" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D71" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E71" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F71" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -4073,10 +4082,10 @@
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="F72" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="G72" t="s">
         <v>4</v>
@@ -4090,19 +4099,19 @@
         <v>73</v>
       </c>
       <c r="C73" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D73" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E73" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F73" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -4113,19 +4122,19 @@
         <v>74</v>
       </c>
       <c r="C74" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D74" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E74" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F74" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -4136,19 +4145,19 @@
         <v>75</v>
       </c>
       <c r="C75" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D75" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E75" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F75" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -4159,19 +4168,19 @@
         <v>76</v>
       </c>
       <c r="C76" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D76" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E76" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F76" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -4182,19 +4191,19 @@
         <v>77</v>
       </c>
       <c r="C77" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D77" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E77" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F77" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="I77" s="2" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -4205,19 +4214,19 @@
         <v>78</v>
       </c>
       <c r="C78" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D78" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E78" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F78" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -4228,19 +4237,19 @@
         <v>79</v>
       </c>
       <c r="C79" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D79" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E79" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F79" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -4257,10 +4266,10 @@
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="F80" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="G80" t="s">
         <v>4</v>
@@ -4274,19 +4283,19 @@
         <v>80</v>
       </c>
       <c r="C81" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D81" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E81" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F81" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -4303,10 +4312,10 @@
         <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="F82" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="G82" t="s">
         <v>4</v>
@@ -4320,19 +4329,19 @@
         <v>81</v>
       </c>
       <c r="C83" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D83" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E83" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="F83" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="I83" s="2" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -4343,19 +4352,19 @@
         <v>82</v>
       </c>
       <c r="C84" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D84" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E84" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="F84" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="I84" s="2" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -4366,19 +4375,19 @@
         <v>83</v>
       </c>
       <c r="C85" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D85" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E85" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F85" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="I85" s="2" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -4389,19 +4398,19 @@
         <v>84</v>
       </c>
       <c r="C86" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D86" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E86" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F86" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="I86" s="2" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
     </row>
     <row r="87" spans="1:9">
@@ -4412,19 +4421,19 @@
         <v>85</v>
       </c>
       <c r="C87" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D87" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E87" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="F87" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="I87" s="2" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
     </row>
     <row r="88" spans="1:9">
@@ -4435,19 +4444,19 @@
         <v>86</v>
       </c>
       <c r="C88" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D88" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E88" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F88" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="I88" s="2" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -4458,19 +4467,19 @@
         <v>87</v>
       </c>
       <c r="C89" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D89" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E89" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F89" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="I89" s="2" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -4481,19 +4490,19 @@
         <v>88</v>
       </c>
       <c r="C90" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D90" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E90" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F90" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -4504,19 +4513,19 @@
         <v>89</v>
       </c>
       <c r="C91" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D91" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E91" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F91" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="I91" s="2" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
     </row>
     <row r="92" spans="1:9">
@@ -4527,19 +4536,19 @@
         <v>90</v>
       </c>
       <c r="C92" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D92" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E92" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F92" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
     </row>
     <row r="93" spans="1:9">
@@ -4550,19 +4559,19 @@
         <v>91</v>
       </c>
       <c r="C93" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D93" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E93" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F93" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="I93" s="2" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
     </row>
     <row r="94" spans="1:9">
@@ -4573,19 +4582,19 @@
         <v>92</v>
       </c>
       <c r="C94" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D94" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E94" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F94" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="I94" s="2" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -4596,19 +4605,19 @@
         <v>93</v>
       </c>
       <c r="C95" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D95" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E95" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F95" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="I95" s="2" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -4619,19 +4628,19 @@
         <v>94</v>
       </c>
       <c r="C96" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D96" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E96" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F96" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="I96" s="2" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -4642,19 +4651,19 @@
         <v>95</v>
       </c>
       <c r="C97" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D97" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E97" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F97" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="I97" s="2" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -4665,19 +4674,19 @@
         <v>96</v>
       </c>
       <c r="C98" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D98" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E98" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F98" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="I98" s="2" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -4688,19 +4697,19 @@
         <v>97</v>
       </c>
       <c r="C99" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D99" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E99" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F99" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="I99" s="2" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
     </row>
     <row r="100" spans="1:9">
@@ -4717,10 +4726,10 @@
         <v>1</v>
       </c>
       <c r="E100" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="F100" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
     </row>
     <row r="101" spans="1:9">
@@ -4731,13 +4740,13 @@
         <v>98</v>
       </c>
       <c r="C101" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D101" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="I101" s="2" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
     </row>
     <row r="102" spans="1:9">
@@ -4754,10 +4763,10 @@
         <v>1</v>
       </c>
       <c r="E102" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="F102" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
     </row>
     <row r="103" spans="1:9">
@@ -4768,13 +4777,13 @@
         <v>99</v>
       </c>
       <c r="C103" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D103" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="I103" s="2" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
     </row>
     <row r="104" spans="1:9">
@@ -4788,16 +4797,16 @@
         <v>5</v>
       </c>
       <c r="D104" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E104" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="F104" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="G104" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="H104" t="s">
         <v>4</v>
@@ -4811,22 +4820,22 @@
         <v>100</v>
       </c>
       <c r="C105" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D105" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E105" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="F105" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="G105" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="I105" s="2" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
     </row>
     <row r="106" spans="1:9">
@@ -4837,22 +4846,22 @@
         <v>101</v>
       </c>
       <c r="C106" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D106" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E106" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="F106" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="G106" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="I106" s="2" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
     </row>
     <row r="107" spans="1:9">
@@ -4863,22 +4872,22 @@
         <v>102</v>
       </c>
       <c r="C107" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D107" t="s">
+        <v>294</v>
+      </c>
+      <c r="E107" t="s">
+        <v>366</v>
+      </c>
+      <c r="F107" t="s">
         <v>293</v>
       </c>
-      <c r="E107" t="s">
-        <v>364</v>
-      </c>
-      <c r="F107" t="s">
-        <v>292</v>
-      </c>
       <c r="G107" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="I107" s="2" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="108" spans="1:9">
@@ -4889,22 +4898,22 @@
         <v>103</v>
       </c>
       <c r="C108" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D108" t="s">
+        <v>294</v>
+      </c>
+      <c r="E108" t="s">
+        <v>366</v>
+      </c>
+      <c r="F108" t="s">
         <v>293</v>
       </c>
-      <c r="E108" t="s">
-        <v>364</v>
-      </c>
-      <c r="F108" t="s">
-        <v>292</v>
-      </c>
       <c r="G108" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="I108" s="2" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
     </row>
     <row r="109" spans="1:9">
@@ -4915,22 +4924,22 @@
         <v>104</v>
       </c>
       <c r="C109" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D109" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E109" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="F109" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="G109" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="I109" s="2" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
     </row>
     <row r="110" spans="1:9">
@@ -4941,22 +4950,22 @@
         <v>105</v>
       </c>
       <c r="C110" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D110" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E110" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="F110" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="G110" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="I110" s="2" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
     </row>
     <row r="111" spans="1:9">
@@ -4967,22 +4976,22 @@
         <v>106</v>
       </c>
       <c r="C111" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D111" t="s">
+        <v>294</v>
+      </c>
+      <c r="E111" t="s">
+        <v>364</v>
+      </c>
+      <c r="F111" t="s">
         <v>293</v>
       </c>
-      <c r="E111" t="s">
-        <v>362</v>
-      </c>
-      <c r="F111" t="s">
-        <v>292</v>
-      </c>
       <c r="G111" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="I111" s="2" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
     </row>
     <row r="112" spans="1:9">
@@ -4993,22 +5002,22 @@
         <v>107</v>
       </c>
       <c r="C112" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D112" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E112" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F112" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="G112" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="I112" s="2" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
     </row>
     <row r="113" spans="1:9">
@@ -5019,22 +5028,22 @@
         <v>108</v>
       </c>
       <c r="C113" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D113" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E113" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="F113" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G113" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="I113" s="2" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
     </row>
     <row r="114" spans="1:9">
@@ -5045,22 +5054,22 @@
         <v>109</v>
       </c>
       <c r="C114" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D114" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E114" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="F114" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G114" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="I114" s="2" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
     </row>
     <row r="115" spans="1:9">
@@ -5071,22 +5080,22 @@
         <v>110</v>
       </c>
       <c r="C115" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D115" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E115" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="F115" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="G115" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="I115" s="2" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
     </row>
     <row r="116" spans="1:9">
@@ -5097,22 +5106,22 @@
         <v>111</v>
       </c>
       <c r="C116" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D116" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E116" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="F116" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="G116" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="I116" s="2" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row r="117" spans="1:9">
@@ -5123,22 +5132,22 @@
         <v>112</v>
       </c>
       <c r="C117" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D117" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E117" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F117" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="G117" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="I117" s="2" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
     </row>
     <row r="118" spans="1:9">
@@ -5149,22 +5158,22 @@
         <v>113</v>
       </c>
       <c r="C118" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D118" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E118" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="F118" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G118" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="I118" s="2" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
     </row>
     <row r="119" spans="1:9">
@@ -5175,22 +5184,22 @@
         <v>114</v>
       </c>
       <c r="C119" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D119" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E119" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="F119" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="G119" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="I119" s="2" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
     </row>
     <row r="120" spans="1:9">
@@ -5204,16 +5213,16 @@
         <v>5</v>
       </c>
       <c r="D120" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E120" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="F120" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="G120" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="H120" t="s">
         <v>4</v>
@@ -5227,22 +5236,22 @@
         <v>115</v>
       </c>
       <c r="C121" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D121" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E121" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="F121" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="G121" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="I121" s="2" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
     </row>
     <row r="122" spans="1:9">
@@ -5253,22 +5262,22 @@
         <v>116</v>
       </c>
       <c r="C122" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D122" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E122" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="F122" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="G122" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="I122" s="2" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
     </row>
     <row r="123" spans="1:9">
@@ -5279,22 +5288,22 @@
         <v>117</v>
       </c>
       <c r="C123" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D123" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E123" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="F123" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="G123" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="I123" s="2" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
     </row>
     <row r="124" spans="1:9">
@@ -5305,22 +5314,22 @@
         <v>118</v>
       </c>
       <c r="C124" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D124" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E124" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="F124" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="G124" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="I124" s="2" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
     </row>
     <row r="125" spans="1:9">
@@ -5331,22 +5340,22 @@
         <v>119</v>
       </c>
       <c r="C125" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D125" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E125" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="F125" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="G125" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="I125" s="2" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
     </row>
     <row r="126" spans="1:9">
@@ -5360,7 +5369,7 @@
         <v>5</v>
       </c>
       <c r="D126" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E126" t="s">
         <v>4</v>
@@ -5374,13 +5383,13 @@
         <v>120</v>
       </c>
       <c r="C127" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D127" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="I127" s="2" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
     </row>
     <row r="128" spans="1:9">
@@ -5394,7 +5403,7 @@
         <v>5</v>
       </c>
       <c r="D128" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E128" t="s">
         <v>4</v>
@@ -5408,13 +5417,13 @@
         <v>121</v>
       </c>
       <c r="C129" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D129" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="I129" s="2" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
     </row>
     <row r="130" spans="1:9">
@@ -5431,7 +5440,7 @@
         <v>1</v>
       </c>
       <c r="E130" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
     <row r="131" spans="1:9">
@@ -5442,13 +5451,13 @@
         <v>122</v>
       </c>
       <c r="C131" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D131" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="I131" s="2" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
     </row>
     <row r="132" spans="1:9">
@@ -5459,13 +5468,13 @@
         <v>123</v>
       </c>
       <c r="C132" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D132" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="I132" s="2" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
     </row>
     <row r="133" spans="1:9">
@@ -5476,13 +5485,13 @@
         <v>124</v>
       </c>
       <c r="C133" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D133" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I133" s="2" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
     </row>
     <row r="134" spans="1:9">
@@ -5493,13 +5502,13 @@
         <v>125</v>
       </c>
       <c r="C134" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D134" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="I134" s="2" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
     </row>
     <row r="135" spans="1:9">
@@ -5510,13 +5519,13 @@
         <v>126</v>
       </c>
       <c r="C135" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D135" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="I135" s="2" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
     </row>
     <row r="136" spans="1:9">
@@ -5527,13 +5536,13 @@
         <v>127</v>
       </c>
       <c r="C136" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D136" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="I136" s="2" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
     </row>
     <row r="137" spans="1:9">
@@ -5544,13 +5553,13 @@
         <v>128</v>
       </c>
       <c r="C137" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D137" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="I137" s="2" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
     </row>
     <row r="138" spans="1:9">
@@ -5561,13 +5570,13 @@
         <v>129</v>
       </c>
       <c r="C138" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D138" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="I138" s="2" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
     </row>
     <row r="139" spans="1:9">
@@ -5578,13 +5587,13 @@
         <v>130</v>
       </c>
       <c r="C139" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D139" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="I139" s="2" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
     </row>
     <row r="140" spans="1:9">
@@ -5595,13 +5604,13 @@
         <v>131</v>
       </c>
       <c r="C140" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D140" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="I140" s="2" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
     </row>
     <row r="141" spans="1:9">
@@ -5612,13 +5621,13 @@
         <v>132</v>
       </c>
       <c r="C141" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D141" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="I141" s="2" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
     </row>
     <row r="142" spans="1:9">
@@ -5629,13 +5638,13 @@
         <v>133</v>
       </c>
       <c r="C142" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D142" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="I142" s="2" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
     </row>
     <row r="143" spans="1:9">
@@ -5646,13 +5655,13 @@
         <v>134</v>
       </c>
       <c r="C143" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D143" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="I143" s="2" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
     </row>
     <row r="144" spans="1:9">
@@ -5663,13 +5672,13 @@
         <v>135</v>
       </c>
       <c r="C144" t="s">
-        <v>249</v>
+        <v>207</v>
       </c>
       <c r="D144" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="I144" s="2" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
     </row>
     <row r="145" spans="1:9">
@@ -5686,7 +5695,7 @@
         <v>312</v>
       </c>
       <c r="I145" s="2" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
     </row>
     <row r="146" spans="1:9">
@@ -5700,10 +5709,10 @@
         <v>251</v>
       </c>
       <c r="D146" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="I146" s="2" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
     </row>
     <row r="147" spans="1:9">
@@ -5717,10 +5726,10 @@
         <v>252</v>
       </c>
       <c r="D147" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="I147" s="2" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
     </row>
     <row r="148" spans="1:9">
@@ -5731,13 +5740,13 @@
         <v>139</v>
       </c>
       <c r="C148" t="s">
-        <v>210</v>
+        <v>253</v>
       </c>
       <c r="D148" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="I148" s="2" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
     </row>
     <row r="149" spans="1:9">
@@ -5748,13 +5757,13 @@
         <v>140</v>
       </c>
       <c r="C149" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D149" t="s">
-        <v>306</v>
+        <v>316</v>
       </c>
       <c r="I149" s="2" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
     </row>
     <row r="150" spans="1:9">
@@ -5765,13 +5774,13 @@
         <v>141</v>
       </c>
       <c r="C150" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="D150" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="I150" s="2" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
     </row>
     <row r="151" spans="1:9">
@@ -5782,13 +5791,13 @@
         <v>142</v>
       </c>
       <c r="C151" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D151" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="I151" s="2" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
     </row>
     <row r="152" spans="1:9">
@@ -5799,13 +5808,13 @@
         <v>143</v>
       </c>
       <c r="C152" t="s">
-        <v>253</v>
+        <v>211</v>
       </c>
       <c r="D152" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="I152" s="2" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
     </row>
     <row r="153" spans="1:9">
@@ -5816,13 +5825,13 @@
         <v>144</v>
       </c>
       <c r="C153" t="s">
-        <v>205</v>
+        <v>254</v>
       </c>
       <c r="D153" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="I153" s="2" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
     </row>
     <row r="154" spans="1:9">
@@ -5833,13 +5842,13 @@
         <v>145</v>
       </c>
       <c r="C154" t="s">
-        <v>254</v>
+        <v>206</v>
       </c>
       <c r="D154" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="I154" s="2" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
     </row>
     <row r="155" spans="1:9">
@@ -5850,13 +5859,13 @@
         <v>146</v>
       </c>
       <c r="C155" t="s">
-        <v>206</v>
+        <v>255</v>
       </c>
       <c r="D155" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="I155" s="2" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
     </row>
     <row r="156" spans="1:9">
@@ -5867,13 +5876,13 @@
         <v>147</v>
       </c>
       <c r="C156" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D156" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I156" s="2" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
     </row>
     <row r="157" spans="1:9">
@@ -5884,13 +5893,13 @@
         <v>148</v>
       </c>
       <c r="C157" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D157" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="I157" s="2" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
     </row>
     <row r="158" spans="1:9">
@@ -5901,13 +5910,13 @@
         <v>149</v>
       </c>
       <c r="C158" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D158" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="I158" s="2" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
     </row>
     <row r="159" spans="1:9">
@@ -5918,13 +5927,13 @@
         <v>150</v>
       </c>
       <c r="C159" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D159" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="I159" s="2" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
     </row>
     <row r="160" spans="1:9">
@@ -5935,13 +5944,13 @@
         <v>151</v>
       </c>
       <c r="C160" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D160" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="I160" s="2" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
     </row>
     <row r="161" spans="1:9">
@@ -5952,13 +5961,13 @@
         <v>152</v>
       </c>
       <c r="C161" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D161" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I161" s="2" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
     </row>
     <row r="162" spans="1:9">
@@ -5969,13 +5978,13 @@
         <v>153</v>
       </c>
       <c r="C162" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D162" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I162" s="2" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
     </row>
     <row r="163" spans="1:9">
@@ -5986,13 +5995,13 @@
         <v>154</v>
       </c>
       <c r="C163" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D163" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="I163" s="2" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
     </row>
     <row r="164" spans="1:9">
@@ -6003,13 +6012,13 @@
         <v>155</v>
       </c>
       <c r="C164" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D164" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="I164" s="2" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
     </row>
     <row r="165" spans="1:9">
@@ -6020,13 +6029,13 @@
         <v>156</v>
       </c>
       <c r="C165" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D165" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="I165" s="2" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
     </row>
     <row r="166" spans="1:9">
@@ -6037,13 +6046,13 @@
         <v>157</v>
       </c>
       <c r="C166" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D166" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="I166" s="2" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
     </row>
     <row r="167" spans="1:9">
@@ -6054,13 +6063,13 @@
         <v>158</v>
       </c>
       <c r="C167" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D167" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="I167" s="2" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
     </row>
     <row r="168" spans="1:9">
@@ -6071,13 +6080,13 @@
         <v>159</v>
       </c>
       <c r="C168" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D168" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="I168" s="2" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
     </row>
     <row r="169" spans="1:9">
@@ -6088,13 +6097,13 @@
         <v>160</v>
       </c>
       <c r="C169" t="s">
-        <v>206</v>
-      </c>
-      <c r="D169" t="s">
-        <v>325</v>
+        <v>207</v>
+      </c>
+      <c r="D169" s="2" t="s">
+        <v>326</v>
       </c>
       <c r="I169" s="2" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
     </row>
     <row r="170" spans="1:9">
@@ -6105,13 +6114,13 @@
         <v>161</v>
       </c>
       <c r="C170" t="s">
-        <v>261</v>
+        <v>207</v>
       </c>
       <c r="D170" t="s">
-        <v>307</v>
+        <v>327</v>
       </c>
       <c r="I170" s="2" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
     </row>
     <row r="171" spans="1:9">
@@ -6122,13 +6131,13 @@
         <v>162</v>
       </c>
       <c r="C171" t="s">
-        <v>207</v>
+        <v>262</v>
       </c>
       <c r="D171" t="s">
-        <v>326</v>
+        <v>308</v>
       </c>
       <c r="I171" s="2" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
     </row>
     <row r="172" spans="1:9">
@@ -6139,13 +6148,13 @@
         <v>163</v>
       </c>
       <c r="C172" t="s">
-        <v>262</v>
+        <v>208</v>
       </c>
       <c r="D172" t="s">
-        <v>311</v>
+        <v>328</v>
       </c>
       <c r="I172" s="2" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
     </row>
     <row r="173" spans="1:9">
@@ -6156,13 +6165,13 @@
         <v>164</v>
       </c>
       <c r="C173" t="s">
-        <v>218</v>
+        <v>263</v>
       </c>
       <c r="D173" t="s">
-        <v>327</v>
+        <v>312</v>
       </c>
       <c r="I173" s="2" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
     </row>
     <row r="174" spans="1:9">
@@ -6173,13 +6182,13 @@
         <v>165</v>
       </c>
       <c r="C174" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="D174" t="s">
-        <v>307</v>
+        <v>329</v>
       </c>
       <c r="I174" s="2" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
     </row>
     <row r="175" spans="1:9">
@@ -6190,13 +6199,13 @@
         <v>166</v>
       </c>
       <c r="C175" t="s">
-        <v>209</v>
+        <v>226</v>
       </c>
       <c r="D175" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="I175" s="2" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
     </row>
     <row r="176" spans="1:9">
@@ -6207,13 +6216,13 @@
         <v>167</v>
       </c>
       <c r="C176" t="s">
-        <v>263</v>
+        <v>210</v>
       </c>
       <c r="D176" t="s">
-        <v>328</v>
+        <v>307</v>
       </c>
       <c r="I176" s="2" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
     </row>
     <row r="177" spans="1:9">
@@ -6227,10 +6236,10 @@
         <v>264</v>
       </c>
       <c r="D177" t="s">
-        <v>310</v>
+        <v>330</v>
       </c>
       <c r="I177" s="2" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
     </row>
     <row r="178" spans="1:9">
@@ -6241,13 +6250,13 @@
         <v>169</v>
       </c>
       <c r="C178" t="s">
-        <v>223</v>
+        <v>265</v>
       </c>
       <c r="D178" t="s">
-        <v>329</v>
+        <v>311</v>
       </c>
       <c r="I178" s="2" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
     </row>
     <row r="179" spans="1:9">
@@ -6258,13 +6267,13 @@
         <v>170</v>
       </c>
       <c r="C179" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D179" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="I179" s="2" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
     </row>
     <row r="180" spans="1:9">
@@ -6275,13 +6284,13 @@
         <v>171</v>
       </c>
       <c r="C180" t="s">
-        <v>265</v>
+        <v>224</v>
       </c>
       <c r="D180" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="I180" s="2" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
     </row>
     <row r="181" spans="1:9">
@@ -6292,13 +6301,13 @@
         <v>172</v>
       </c>
       <c r="C181" t="s">
-        <v>223</v>
+        <v>266</v>
       </c>
       <c r="D181" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="I181" s="2" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
     </row>
     <row r="182" spans="1:9">
@@ -6309,13 +6318,13 @@
         <v>173</v>
       </c>
       <c r="C182" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="D182" t="s">
-        <v>307</v>
+        <v>333</v>
       </c>
       <c r="I182" s="2" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
     </row>
     <row r="183" spans="1:9">
@@ -6326,13 +6335,13 @@
         <v>174</v>
       </c>
       <c r="C183" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="D183" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I183" s="2" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
     </row>
     <row r="184" spans="1:9">
@@ -6343,13 +6352,13 @@
         <v>175</v>
       </c>
       <c r="C184" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D184" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="I184" s="2" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
     </row>
     <row r="185" spans="1:9">
@@ -6360,13 +6369,13 @@
         <v>176</v>
       </c>
       <c r="C185" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="D185" t="s">
         <v>307</v>
       </c>
       <c r="I185" s="2" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
     </row>
     <row r="186" spans="1:9">
@@ -6377,13 +6386,13 @@
         <v>177</v>
       </c>
       <c r="C186" t="s">
-        <v>206</v>
+        <v>224</v>
       </c>
       <c r="D186" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I186" s="2" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
     </row>
     <row r="187" spans="1:9">
@@ -6394,13 +6403,13 @@
         <v>178</v>
       </c>
       <c r="C187" t="s">
-        <v>266</v>
+        <v>207</v>
       </c>
       <c r="D187" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I187" s="2" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
     </row>
     <row r="188" spans="1:9">
@@ -6408,16 +6417,16 @@
         <v>186</v>
       </c>
       <c r="B188" t="s">
-        <v>0</v>
+        <v>179</v>
       </c>
       <c r="C188" t="s">
-        <v>5</v>
+        <v>267</v>
       </c>
       <c r="D188" t="s">
-        <v>1</v>
-      </c>
-      <c r="E188" t="s">
-        <v>341</v>
+        <v>308</v>
+      </c>
+      <c r="I188" s="2" t="s">
+        <v>668</v>
       </c>
     </row>
     <row r="189" spans="1:9">
@@ -6425,16 +6434,16 @@
         <v>187</v>
       </c>
       <c r="B189" t="s">
-        <v>179</v>
+        <v>0</v>
       </c>
       <c r="C189" t="s">
-        <v>267</v>
+        <v>5</v>
       </c>
       <c r="D189" t="s">
-        <v>332</v>
-      </c>
-      <c r="I189" s="2" t="s">
-        <v>666</v>
+        <v>1</v>
+      </c>
+      <c r="E189" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="190" spans="1:9">
@@ -6448,10 +6457,10 @@
         <v>268</v>
       </c>
       <c r="D190" t="s">
-        <v>311</v>
+        <v>334</v>
       </c>
       <c r="I190" s="2" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
     </row>
     <row r="191" spans="1:9">
@@ -6462,13 +6471,13 @@
         <v>181</v>
       </c>
       <c r="C191" t="s">
-        <v>213</v>
+        <v>269</v>
       </c>
       <c r="D191" t="s">
-        <v>333</v>
+        <v>312</v>
       </c>
       <c r="I191" s="2" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
     </row>
     <row r="192" spans="1:9">
@@ -6479,13 +6488,13 @@
         <v>182</v>
       </c>
       <c r="C192" t="s">
-        <v>269</v>
+        <v>214</v>
       </c>
       <c r="D192" t="s">
-        <v>312</v>
+        <v>335</v>
       </c>
       <c r="I192" s="2" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
     </row>
     <row r="193" spans="1:9">
@@ -6496,13 +6505,13 @@
         <v>183</v>
       </c>
       <c r="C193" t="s">
-        <v>213</v>
+        <v>270</v>
       </c>
       <c r="D193" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="I193" s="2" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
     </row>
     <row r="194" spans="1:9">
@@ -6513,13 +6522,13 @@
         <v>184</v>
       </c>
       <c r="C194" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D194" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="I194" s="2" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
     </row>
     <row r="195" spans="1:9">
@@ -6530,13 +6539,13 @@
         <v>185</v>
       </c>
       <c r="C195" t="s">
-        <v>270</v>
+        <v>214</v>
       </c>
       <c r="D195" t="s">
-        <v>334</v>
+        <v>307</v>
       </c>
       <c r="I195" s="2" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
     </row>
     <row r="196" spans="1:9">
@@ -6550,10 +6559,10 @@
         <v>271</v>
       </c>
       <c r="D196" t="s">
-        <v>311</v>
+        <v>336</v>
       </c>
       <c r="I196" s="2" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
     </row>
     <row r="197" spans="1:9">
@@ -6567,10 +6576,10 @@
         <v>272</v>
       </c>
       <c r="D197" t="s">
-        <v>333</v>
+        <v>312</v>
       </c>
       <c r="I197" s="2" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
     </row>
     <row r="198" spans="1:9">
@@ -6581,13 +6590,13 @@
         <v>188</v>
       </c>
       <c r="C198" t="s">
-        <v>216</v>
+        <v>273</v>
       </c>
       <c r="D198" t="s">
-        <v>312</v>
+        <v>335</v>
       </c>
       <c r="I198" s="2" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
     </row>
     <row r="199" spans="1:9">
@@ -6598,10 +6607,13 @@
         <v>189</v>
       </c>
       <c r="C199" t="s">
-        <v>273</v>
+        <v>217</v>
       </c>
       <c r="D199" t="s">
-        <v>307</v>
+        <v>314</v>
+      </c>
+      <c r="I199" s="2" t="s">
+        <v>678</v>
       </c>
     </row>
     <row r="200" spans="1:9">
@@ -6615,7 +6627,7 @@
         <v>274</v>
       </c>
       <c r="D200" t="s">
-        <v>333</v>
+        <v>308</v>
       </c>
     </row>
     <row r="201" spans="1:9">
@@ -6623,16 +6635,13 @@
         <v>199</v>
       </c>
       <c r="B201" t="s">
-        <v>0</v>
+        <v>191</v>
       </c>
       <c r="C201" t="s">
-        <v>5</v>
+        <v>275</v>
       </c>
       <c r="D201" t="s">
-        <v>1</v>
-      </c>
-      <c r="E201" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
     </row>
     <row r="202" spans="1:9">
@@ -6640,13 +6649,16 @@
         <v>200</v>
       </c>
       <c r="B202" t="s">
-        <v>191</v>
+        <v>0</v>
       </c>
       <c r="C202" t="s">
-        <v>275</v>
+        <v>5</v>
       </c>
       <c r="D202" t="s">
-        <v>335</v>
+        <v>1</v>
+      </c>
+      <c r="E202" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="203" spans="1:9">
@@ -6657,10 +6669,10 @@
         <v>192</v>
       </c>
       <c r="C203" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D203" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="204" spans="1:9">
@@ -6671,10 +6683,10 @@
         <v>193</v>
       </c>
       <c r="C204" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D204" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="205" spans="1:9">
@@ -6685,10 +6697,10 @@
         <v>194</v>
       </c>
       <c r="C205" t="s">
-        <v>224</v>
+        <v>276</v>
       </c>
       <c r="D205" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
     </row>
     <row r="206" spans="1:9">
@@ -6699,10 +6711,10 @@
         <v>195</v>
       </c>
       <c r="C206" t="s">
-        <v>276</v>
+        <v>225</v>
       </c>
       <c r="D206" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="207" spans="1:9">
@@ -6713,10 +6725,10 @@
         <v>196</v>
       </c>
       <c r="C207" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D207" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="208" spans="1:9">
@@ -6727,10 +6739,10 @@
         <v>197</v>
       </c>
       <c r="C208" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D208" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="209" spans="1:5">
@@ -6738,13 +6750,13 @@
         <v>207</v>
       </c>
       <c r="B209" t="s">
-        <v>0</v>
+        <v>198</v>
       </c>
       <c r="C209" t="s">
-        <v>5</v>
+        <v>278</v>
       </c>
       <c r="D209" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="210" spans="1:5">
@@ -6758,10 +6770,7 @@
         <v>5</v>
       </c>
       <c r="D210" t="s">
-        <v>342</v>
-      </c>
-      <c r="E210" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
     <row r="211" spans="1:5">
@@ -6769,12 +6778,15 @@
         <v>209</v>
       </c>
       <c r="B211" t="s">
-        <v>198</v>
+        <v>0</v>
       </c>
       <c r="C211" t="s">
-        <v>278</v>
+        <v>5</v>
       </c>
       <c r="D211" t="s">
+        <v>344</v>
+      </c>
+      <c r="E211" t="s">
         <v>343</v>
       </c>
     </row>
@@ -6789,7 +6801,7 @@
         <v>279</v>
       </c>
       <c r="D212" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="213" spans="1:5">
@@ -6797,16 +6809,13 @@
         <v>211</v>
       </c>
       <c r="B213" t="s">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="C213" t="s">
-        <v>5</v>
+        <v>280</v>
       </c>
       <c r="D213" t="s">
-        <v>342</v>
-      </c>
-      <c r="E213" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
     </row>
     <row r="214" spans="1:5">
@@ -6814,13 +6823,16 @@
         <v>212</v>
       </c>
       <c r="B214" t="s">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="C214" t="s">
-        <v>280</v>
+        <v>5</v>
       </c>
       <c r="D214" t="s">
-        <v>345</v>
+        <v>344</v>
+      </c>
+      <c r="E214" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="215" spans="1:5">
@@ -6834,7 +6846,7 @@
         <v>281</v>
       </c>
       <c r="D215" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
     </row>
     <row r="216" spans="1:5">
@@ -6845,10 +6857,10 @@
         <v>202</v>
       </c>
       <c r="C216" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D216" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="217" spans="1:5">
@@ -6859,10 +6871,10 @@
         <v>203</v>
       </c>
       <c r="C217" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D217" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="218" spans="1:5">
@@ -6873,10 +6885,24 @@
         <v>204</v>
       </c>
       <c r="C218" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D218" t="s">
-        <v>345</v>
+        <v>349</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5">
+      <c r="A219" s="1">
+        <v>217</v>
+      </c>
+      <c r="B219" t="s">
+        <v>205</v>
+      </c>
+      <c r="C219" t="s">
+        <v>282</v>
+      </c>
+      <c r="D219" t="s">
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -7033,35 +7059,37 @@
     <hyperlink ref="I166" r:id="rId150"/>
     <hyperlink ref="I167" r:id="rId151"/>
     <hyperlink ref="I168" r:id="rId152"/>
-    <hyperlink ref="I169" r:id="rId153"/>
-    <hyperlink ref="I170" r:id="rId154"/>
-    <hyperlink ref="I171" r:id="rId155"/>
-    <hyperlink ref="I172" r:id="rId156"/>
-    <hyperlink ref="I173" r:id="rId157"/>
-    <hyperlink ref="I174" r:id="rId158"/>
-    <hyperlink ref="I175" r:id="rId159"/>
-    <hyperlink ref="I176" r:id="rId160"/>
-    <hyperlink ref="I177" r:id="rId161"/>
-    <hyperlink ref="I178" r:id="rId162"/>
-    <hyperlink ref="I179" r:id="rId163"/>
-    <hyperlink ref="I180" r:id="rId164"/>
-    <hyperlink ref="I181" r:id="rId165"/>
-    <hyperlink ref="I182" r:id="rId166"/>
-    <hyperlink ref="I183" r:id="rId167"/>
-    <hyperlink ref="I184" r:id="rId168"/>
-    <hyperlink ref="I185" r:id="rId169"/>
-    <hyperlink ref="I186" r:id="rId170"/>
-    <hyperlink ref="I187" r:id="rId171"/>
-    <hyperlink ref="I189" r:id="rId172"/>
-    <hyperlink ref="I190" r:id="rId173"/>
-    <hyperlink ref="I191" r:id="rId174"/>
-    <hyperlink ref="I192" r:id="rId175"/>
-    <hyperlink ref="I193" r:id="rId176"/>
-    <hyperlink ref="I194" r:id="rId177"/>
-    <hyperlink ref="I195" r:id="rId178"/>
-    <hyperlink ref="I196" r:id="rId179"/>
-    <hyperlink ref="I197" r:id="rId180"/>
-    <hyperlink ref="I198" r:id="rId181"/>
+    <hyperlink ref="D169" r:id="rId153"/>
+    <hyperlink ref="I169" r:id="rId154"/>
+    <hyperlink ref="I170" r:id="rId155"/>
+    <hyperlink ref="I171" r:id="rId156"/>
+    <hyperlink ref="I172" r:id="rId157"/>
+    <hyperlink ref="I173" r:id="rId158"/>
+    <hyperlink ref="I174" r:id="rId159"/>
+    <hyperlink ref="I175" r:id="rId160"/>
+    <hyperlink ref="I176" r:id="rId161"/>
+    <hyperlink ref="I177" r:id="rId162"/>
+    <hyperlink ref="I178" r:id="rId163"/>
+    <hyperlink ref="I179" r:id="rId164"/>
+    <hyperlink ref="I180" r:id="rId165"/>
+    <hyperlink ref="I181" r:id="rId166"/>
+    <hyperlink ref="I182" r:id="rId167"/>
+    <hyperlink ref="I183" r:id="rId168"/>
+    <hyperlink ref="I184" r:id="rId169"/>
+    <hyperlink ref="I185" r:id="rId170"/>
+    <hyperlink ref="I186" r:id="rId171"/>
+    <hyperlink ref="I187" r:id="rId172"/>
+    <hyperlink ref="I188" r:id="rId173"/>
+    <hyperlink ref="I190" r:id="rId174"/>
+    <hyperlink ref="I191" r:id="rId175"/>
+    <hyperlink ref="I192" r:id="rId176"/>
+    <hyperlink ref="I193" r:id="rId177"/>
+    <hyperlink ref="I194" r:id="rId178"/>
+    <hyperlink ref="I195" r:id="rId179"/>
+    <hyperlink ref="I196" r:id="rId180"/>
+    <hyperlink ref="I197" r:id="rId181"/>
+    <hyperlink ref="I198" r:id="rId182"/>
+    <hyperlink ref="I199" r:id="rId183"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed issue with table
</commit_message>
<xml_diff>
--- a/Data/Weapons.xlsx
+++ b/Data/Weapons.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="678">
   <si>
     <t>Name</t>
   </si>
@@ -956,7 +956,7 @@
     <t>Confirmed on Reddit</t>
   </si>
   <si>
-    <t>Facebook, Twitter 1, Twitter 2</t>
+    <t>Facebook, Twitter 1, Twitter 2 Youtube</t>
   </si>
   <si>
     <t>Confirmed on russian audiopodcast with BSG</t>
@@ -996,7 +996,7 @@
     <t>Confirmed, but not revealed</t>
   </si>
   <si>
-    <t>https://twitter.com/bstategames/status/1390304853033816069?s=20</t>
+    <t>Twitter</t>
   </si>
   <si>
     <t>Confirmed on Reddit and an Instagram video</t>
@@ -1032,9 +1032,6 @@
   </si>
   <si>
     <t>Confirmed on TarkovTV DevBlog № 4</t>
-  </si>
-  <si>
-    <t>Twitter</t>
   </si>
   <si>
     <t>Temporarily removed due to bugs</t>
@@ -2472,13 +2469,13 @@
         <v>283</v>
       </c>
       <c r="E2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2495,13 +2492,13 @@
         <v>284</v>
       </c>
       <c r="E3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -2518,13 +2515,13 @@
         <v>284</v>
       </c>
       <c r="E4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -2541,13 +2538,13 @@
         <v>284</v>
       </c>
       <c r="E5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -2564,13 +2561,13 @@
         <v>284</v>
       </c>
       <c r="E6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -2587,13 +2584,13 @@
         <v>284</v>
       </c>
       <c r="E7" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F7" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -2610,13 +2607,13 @@
         <v>284</v>
       </c>
       <c r="E8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -2633,13 +2630,13 @@
         <v>284</v>
       </c>
       <c r="E9" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F9" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -2656,13 +2653,13 @@
         <v>284</v>
       </c>
       <c r="E10" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F10" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -2679,13 +2676,13 @@
         <v>284</v>
       </c>
       <c r="E11" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -2702,13 +2699,13 @@
         <v>284</v>
       </c>
       <c r="E12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -2725,13 +2722,13 @@
         <v>284</v>
       </c>
       <c r="E13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F13" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -2748,13 +2745,13 @@
         <v>284</v>
       </c>
       <c r="E14" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F14" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -2771,13 +2768,13 @@
         <v>284</v>
       </c>
       <c r="E15" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F15" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -2794,13 +2791,13 @@
         <v>284</v>
       </c>
       <c r="E16" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F16" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -2817,13 +2814,13 @@
         <v>284</v>
       </c>
       <c r="E17" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F17" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -2840,13 +2837,13 @@
         <v>284</v>
       </c>
       <c r="E18" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F18" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -2863,13 +2860,13 @@
         <v>284</v>
       </c>
       <c r="E19" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F19" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -2886,13 +2883,13 @@
         <v>284</v>
       </c>
       <c r="E20" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F20" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -2909,13 +2906,13 @@
         <v>284</v>
       </c>
       <c r="E21" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F21" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -2932,13 +2929,13 @@
         <v>284</v>
       </c>
       <c r="E22" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F22" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -2955,13 +2952,13 @@
         <v>284</v>
       </c>
       <c r="E23" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F23" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -2978,13 +2975,13 @@
         <v>284</v>
       </c>
       <c r="E24" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F24" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -3001,13 +2998,13 @@
         <v>283</v>
       </c>
       <c r="E25" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F25" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -3024,13 +3021,13 @@
         <v>284</v>
       </c>
       <c r="E26" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F26" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -3047,13 +3044,13 @@
         <v>284</v>
       </c>
       <c r="E27" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F27" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -3070,13 +3067,13 @@
         <v>284</v>
       </c>
       <c r="E28" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F28" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -3093,13 +3090,13 @@
         <v>283</v>
       </c>
       <c r="E29" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F29" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -3116,13 +3113,13 @@
         <v>283</v>
       </c>
       <c r="E30" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F30" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -3139,13 +3136,13 @@
         <v>283</v>
       </c>
       <c r="E31" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F31" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -3162,10 +3159,10 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F32" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G32" t="s">
         <v>4</v>
@@ -3185,13 +3182,13 @@
         <v>283</v>
       </c>
       <c r="E33" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F33" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -3208,13 +3205,13 @@
         <v>283</v>
       </c>
       <c r="E34" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F34" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -3231,13 +3228,13 @@
         <v>283</v>
       </c>
       <c r="E35" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F35" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -3254,10 +3251,10 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F36" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G36" t="s">
         <v>4</v>
@@ -3277,13 +3274,13 @@
         <v>284</v>
       </c>
       <c r="E37" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F37" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -3300,10 +3297,10 @@
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F38" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G38" t="s">
         <v>4</v>
@@ -3323,13 +3320,13 @@
         <v>285</v>
       </c>
       <c r="E39" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F39" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -3346,13 +3343,13 @@
         <v>285</v>
       </c>
       <c r="E40" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F40" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -3369,13 +3366,13 @@
         <v>284</v>
       </c>
       <c r="E41" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F41" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -3392,13 +3389,13 @@
         <v>284</v>
       </c>
       <c r="E42" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F42" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -3415,13 +3412,13 @@
         <v>284</v>
       </c>
       <c r="E43" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F43" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -3438,13 +3435,13 @@
         <v>284</v>
       </c>
       <c r="E44" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F44" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -3461,13 +3458,13 @@
         <v>284</v>
       </c>
       <c r="E45" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F45" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -3484,13 +3481,13 @@
         <v>284</v>
       </c>
       <c r="E46" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F46" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -3507,13 +3504,13 @@
         <v>284</v>
       </c>
       <c r="E47" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F47" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -3530,13 +3527,13 @@
         <v>284</v>
       </c>
       <c r="E48" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F48" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -3553,13 +3550,13 @@
         <v>284</v>
       </c>
       <c r="E49" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F49" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -3576,13 +3573,13 @@
         <v>284</v>
       </c>
       <c r="E50" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F50" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -3599,13 +3596,13 @@
         <v>284</v>
       </c>
       <c r="E51" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F51" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -3622,13 +3619,13 @@
         <v>283</v>
       </c>
       <c r="E52" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F52" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -3645,13 +3642,13 @@
         <v>283</v>
       </c>
       <c r="E53" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F53" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -3668,13 +3665,13 @@
         <v>284</v>
       </c>
       <c r="E54" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F54" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -3691,13 +3688,13 @@
         <v>286</v>
       </c>
       <c r="E55" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F55" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -3714,13 +3711,13 @@
         <v>286</v>
       </c>
       <c r="E56" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F56" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -3737,10 +3734,10 @@
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F57" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G57" t="s">
         <v>4</v>
@@ -3763,10 +3760,10 @@
         <v>233</v>
       </c>
       <c r="F58" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -3786,10 +3783,10 @@
         <v>233</v>
       </c>
       <c r="F59" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -3809,10 +3806,10 @@
         <v>233</v>
       </c>
       <c r="F60" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -3829,13 +3826,13 @@
         <v>283</v>
       </c>
       <c r="E61" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F61" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -3852,13 +3849,13 @@
         <v>283</v>
       </c>
       <c r="E62" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F62" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -3878,10 +3875,10 @@
         <v>233</v>
       </c>
       <c r="F63" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -3901,10 +3898,10 @@
         <v>233</v>
       </c>
       <c r="F64" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -3921,10 +3918,10 @@
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F65" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G65" t="s">
         <v>4</v>
@@ -3944,13 +3941,13 @@
         <v>283</v>
       </c>
       <c r="E66" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F66" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -3970,10 +3967,10 @@
         <v>233</v>
       </c>
       <c r="F67" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -3990,13 +3987,13 @@
         <v>283</v>
       </c>
       <c r="E68" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F68" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -4013,13 +4010,13 @@
         <v>283</v>
       </c>
       <c r="E69" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F69" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -4036,13 +4033,13 @@
         <v>283</v>
       </c>
       <c r="E70" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F70" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -4059,13 +4056,13 @@
         <v>284</v>
       </c>
       <c r="E71" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F71" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -4082,10 +4079,10 @@
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F72" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G72" t="s">
         <v>4</v>
@@ -4108,10 +4105,10 @@
         <v>233</v>
       </c>
       <c r="F73" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -4131,10 +4128,10 @@
         <v>233</v>
       </c>
       <c r="F74" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -4154,10 +4151,10 @@
         <v>233</v>
       </c>
       <c r="F75" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -4177,10 +4174,10 @@
         <v>233</v>
       </c>
       <c r="F76" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -4200,10 +4197,10 @@
         <v>233</v>
       </c>
       <c r="F77" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="I77" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -4223,10 +4220,10 @@
         <v>233</v>
       </c>
       <c r="F78" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -4246,10 +4243,10 @@
         <v>233</v>
       </c>
       <c r="F79" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -4266,10 +4263,10 @@
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F80" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G80" t="s">
         <v>4</v>
@@ -4292,10 +4289,10 @@
         <v>233</v>
       </c>
       <c r="F81" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -4312,10 +4309,10 @@
         <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F82" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G82" t="s">
         <v>4</v>
@@ -4335,13 +4332,13 @@
         <v>284</v>
       </c>
       <c r="E83" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F83" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="I83" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -4358,13 +4355,13 @@
         <v>284</v>
       </c>
       <c r="E84" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F84" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I84" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -4384,10 +4381,10 @@
         <v>233</v>
       </c>
       <c r="F85" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="I85" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -4407,10 +4404,10 @@
         <v>233</v>
       </c>
       <c r="F86" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I86" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="87" spans="1:9">
@@ -4427,13 +4424,13 @@
         <v>284</v>
       </c>
       <c r="E87" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F87" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="I87" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="88" spans="1:9">
@@ -4453,10 +4450,10 @@
         <v>233</v>
       </c>
       <c r="F88" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="I88" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -4476,10 +4473,10 @@
         <v>233</v>
       </c>
       <c r="F89" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="I89" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -4499,10 +4496,10 @@
         <v>233</v>
       </c>
       <c r="F90" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -4522,10 +4519,10 @@
         <v>233</v>
       </c>
       <c r="F91" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="I91" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="92" spans="1:9">
@@ -4545,10 +4542,10 @@
         <v>233</v>
       </c>
       <c r="F92" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="93" spans="1:9">
@@ -4568,10 +4565,10 @@
         <v>233</v>
       </c>
       <c r="F93" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I93" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="94" spans="1:9">
@@ -4591,10 +4588,10 @@
         <v>233</v>
       </c>
       <c r="F94" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="I94" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -4614,10 +4611,10 @@
         <v>233</v>
       </c>
       <c r="F95" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I95" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -4637,10 +4634,10 @@
         <v>233</v>
       </c>
       <c r="F96" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I96" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -4660,10 +4657,10 @@
         <v>233</v>
       </c>
       <c r="F97" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I97" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -4683,10 +4680,10 @@
         <v>233</v>
       </c>
       <c r="F98" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I98" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -4706,10 +4703,10 @@
         <v>233</v>
       </c>
       <c r="F99" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="I99" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="100" spans="1:9">
@@ -4726,10 +4723,10 @@
         <v>1</v>
       </c>
       <c r="E100" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F100" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="101" spans="1:9">
@@ -4746,7 +4743,7 @@
         <v>290</v>
       </c>
       <c r="I101" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="102" spans="1:9">
@@ -4763,10 +4760,10 @@
         <v>1</v>
       </c>
       <c r="E102" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F102" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="103" spans="1:9">
@@ -4783,7 +4780,7 @@
         <v>290</v>
       </c>
       <c r="I103" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="104" spans="1:9">
@@ -4800,13 +4797,13 @@
         <v>291</v>
       </c>
       <c r="E104" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F104" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G104" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="H104" t="s">
         <v>4</v>
@@ -4826,16 +4823,16 @@
         <v>292</v>
       </c>
       <c r="E105" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F105" t="s">
         <v>295</v>
       </c>
       <c r="G105" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="I105" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="106" spans="1:9">
@@ -4852,16 +4849,16 @@
         <v>293</v>
       </c>
       <c r="E106" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F106" t="s">
         <v>295</v>
       </c>
       <c r="G106" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="I106" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="107" spans="1:9">
@@ -4878,16 +4875,16 @@
         <v>294</v>
       </c>
       <c r="E107" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F107" t="s">
         <v>293</v>
       </c>
       <c r="G107" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="I107" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="108" spans="1:9">
@@ -4904,16 +4901,16 @@
         <v>294</v>
       </c>
       <c r="E108" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F108" t="s">
         <v>293</v>
       </c>
       <c r="G108" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="I108" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="109" spans="1:9">
@@ -4930,16 +4927,16 @@
         <v>293</v>
       </c>
       <c r="E109" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F109" t="s">
         <v>297</v>
       </c>
       <c r="G109" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="I109" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="110" spans="1:9">
@@ -4956,16 +4953,16 @@
         <v>293</v>
       </c>
       <c r="E110" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F110" t="s">
         <v>295</v>
       </c>
       <c r="G110" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I110" s="2" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="111" spans="1:9">
@@ -4982,16 +4979,16 @@
         <v>294</v>
       </c>
       <c r="E111" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F111" t="s">
         <v>293</v>
       </c>
       <c r="G111" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="I111" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="112" spans="1:9">
@@ -5014,10 +5011,10 @@
         <v>295</v>
       </c>
       <c r="G112" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I112" s="2" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="113" spans="1:9">
@@ -5034,16 +5031,16 @@
         <v>295</v>
       </c>
       <c r="E113" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F113" t="s">
         <v>298</v>
       </c>
       <c r="G113" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I113" s="2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="114" spans="1:9">
@@ -5060,16 +5057,16 @@
         <v>295</v>
       </c>
       <c r="E114" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F114" t="s">
         <v>298</v>
       </c>
       <c r="G114" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="I114" s="2" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="115" spans="1:9">
@@ -5086,16 +5083,16 @@
         <v>296</v>
       </c>
       <c r="E115" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F115" t="s">
         <v>296</v>
       </c>
       <c r="G115" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I115" s="2" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="116" spans="1:9">
@@ -5112,16 +5109,16 @@
         <v>297</v>
       </c>
       <c r="E116" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F116" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G116" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I116" s="2" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="117" spans="1:9">
@@ -5141,13 +5138,13 @@
         <v>233</v>
       </c>
       <c r="F117" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G117" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I117" s="2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="118" spans="1:9">
@@ -5164,16 +5161,16 @@
         <v>295</v>
       </c>
       <c r="E118" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F118" t="s">
         <v>298</v>
       </c>
       <c r="G118" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="I118" s="2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="119" spans="1:9">
@@ -5190,16 +5187,16 @@
         <v>297</v>
       </c>
       <c r="E119" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F119" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G119" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I119" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="120" spans="1:9">
@@ -5216,13 +5213,13 @@
         <v>299</v>
       </c>
       <c r="E120" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F120" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G120" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H120" t="s">
         <v>4</v>
@@ -5242,16 +5239,16 @@
         <v>300</v>
       </c>
       <c r="E121" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F121" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G121" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I121" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="122" spans="1:9">
@@ -5268,16 +5265,16 @@
         <v>301</v>
       </c>
       <c r="E122" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F122" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G122" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="I122" s="2" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="123" spans="1:9">
@@ -5294,16 +5291,16 @@
         <v>300</v>
       </c>
       <c r="E123" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F123" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G123" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I123" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="124" spans="1:9">
@@ -5320,16 +5317,16 @@
         <v>302</v>
       </c>
       <c r="E124" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F124" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G124" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="I124" s="2" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="125" spans="1:9">
@@ -5346,16 +5343,16 @@
         <v>303</v>
       </c>
       <c r="E125" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F125" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G125" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="I125" s="2" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="126" spans="1:9">
@@ -5389,7 +5386,7 @@
         <v>304</v>
       </c>
       <c r="I127" s="2" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="128" spans="1:9">
@@ -5423,7 +5420,7 @@
         <v>305</v>
       </c>
       <c r="I129" s="2" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="130" spans="1:9">
@@ -5440,7 +5437,7 @@
         <v>1</v>
       </c>
       <c r="E130" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="131" spans="1:9">
@@ -5457,7 +5454,7 @@
         <v>306</v>
       </c>
       <c r="I131" s="2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="132" spans="1:9">
@@ -5474,7 +5471,7 @@
         <v>307</v>
       </c>
       <c r="I132" s="2" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="133" spans="1:9">
@@ -5491,7 +5488,7 @@
         <v>308</v>
       </c>
       <c r="I133" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="134" spans="1:9">
@@ -5508,7 +5505,7 @@
         <v>307</v>
       </c>
       <c r="I134" s="2" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="135" spans="1:9">
@@ -5525,7 +5522,7 @@
         <v>309</v>
       </c>
       <c r="I135" s="2" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="136" spans="1:9">
@@ -5542,7 +5539,7 @@
         <v>309</v>
       </c>
       <c r="I136" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="137" spans="1:9">
@@ -5559,7 +5556,7 @@
         <v>310</v>
       </c>
       <c r="I137" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="138" spans="1:9">
@@ -5576,7 +5573,7 @@
         <v>311</v>
       </c>
       <c r="I138" s="2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="139" spans="1:9">
@@ -5593,7 +5590,7 @@
         <v>312</v>
       </c>
       <c r="I139" s="2" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="140" spans="1:9">
@@ -5610,7 +5607,7 @@
         <v>311</v>
       </c>
       <c r="I140" s="2" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="141" spans="1:9">
@@ -5627,7 +5624,7 @@
         <v>311</v>
       </c>
       <c r="I141" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="142" spans="1:9">
@@ -5644,7 +5641,7 @@
         <v>312</v>
       </c>
       <c r="I142" s="2" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="143" spans="1:9">
@@ -5661,7 +5658,7 @@
         <v>307</v>
       </c>
       <c r="I143" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="144" spans="1:9">
@@ -5678,7 +5675,7 @@
         <v>313</v>
       </c>
       <c r="I144" s="2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="145" spans="1:9">
@@ -5695,7 +5692,7 @@
         <v>312</v>
       </c>
       <c r="I145" s="2" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="146" spans="1:9">
@@ -5712,7 +5709,7 @@
         <v>314</v>
       </c>
       <c r="I146" s="2" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="147" spans="1:9">
@@ -5729,7 +5726,7 @@
         <v>307</v>
       </c>
       <c r="I147" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="148" spans="1:9">
@@ -5746,7 +5743,7 @@
         <v>315</v>
       </c>
       <c r="I148" s="2" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="149" spans="1:9">
@@ -5763,7 +5760,7 @@
         <v>316</v>
       </c>
       <c r="I149" s="2" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="150" spans="1:9">
@@ -5780,7 +5777,7 @@
         <v>307</v>
       </c>
       <c r="I150" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="151" spans="1:9">
@@ -5797,7 +5794,7 @@
         <v>307</v>
       </c>
       <c r="I151" s="2" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="152" spans="1:9">
@@ -5814,7 +5811,7 @@
         <v>317</v>
       </c>
       <c r="I152" s="2" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="153" spans="1:9">
@@ -5831,7 +5828,7 @@
         <v>318</v>
       </c>
       <c r="I153" s="2" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="154" spans="1:9">
@@ -5848,7 +5845,7 @@
         <v>311</v>
       </c>
       <c r="I154" s="2" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="155" spans="1:9">
@@ -5865,7 +5862,7 @@
         <v>319</v>
       </c>
       <c r="I155" s="2" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="156" spans="1:9">
@@ -5882,7 +5879,7 @@
         <v>308</v>
       </c>
       <c r="I156" s="2" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="157" spans="1:9">
@@ -5899,7 +5896,7 @@
         <v>307</v>
       </c>
       <c r="I157" s="2" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="158" spans="1:9">
@@ -5916,7 +5913,7 @@
         <v>320</v>
       </c>
       <c r="I158" s="2" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="159" spans="1:9">
@@ -5933,7 +5930,7 @@
         <v>321</v>
       </c>
       <c r="I159" s="2" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="160" spans="1:9">
@@ -5950,7 +5947,7 @@
         <v>322</v>
       </c>
       <c r="I160" s="2" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="161" spans="1:9">
@@ -5967,7 +5964,7 @@
         <v>308</v>
       </c>
       <c r="I161" s="2" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="162" spans="1:9">
@@ -5984,7 +5981,7 @@
         <v>308</v>
       </c>
       <c r="I162" s="2" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="163" spans="1:9">
@@ -6001,7 +5998,7 @@
         <v>323</v>
       </c>
       <c r="I163" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="164" spans="1:9">
@@ -6018,7 +6015,7 @@
         <v>324</v>
       </c>
       <c r="I164" s="2" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="165" spans="1:9">
@@ -6035,7 +6032,7 @@
         <v>307</v>
       </c>
       <c r="I165" s="2" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="166" spans="1:9">
@@ -6052,7 +6049,7 @@
         <v>325</v>
       </c>
       <c r="I166" s="2" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="167" spans="1:9">
@@ -6069,7 +6066,7 @@
         <v>325</v>
       </c>
       <c r="I167" s="2" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="168" spans="1:9">
@@ -6086,7 +6083,7 @@
         <v>307</v>
       </c>
       <c r="I168" s="2" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="169" spans="1:9">
@@ -6099,11 +6096,11 @@
       <c r="C169" t="s">
         <v>207</v>
       </c>
-      <c r="D169" s="2" t="s">
+      <c r="D169" t="s">
         <v>326</v>
       </c>
       <c r="I169" s="2" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="170" spans="1:9">
@@ -6120,7 +6117,7 @@
         <v>327</v>
       </c>
       <c r="I170" s="2" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="171" spans="1:9">
@@ -6137,7 +6134,7 @@
         <v>308</v>
       </c>
       <c r="I171" s="2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="172" spans="1:9">
@@ -6154,7 +6151,7 @@
         <v>328</v>
       </c>
       <c r="I172" s="2" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="173" spans="1:9">
@@ -6171,7 +6168,7 @@
         <v>312</v>
       </c>
       <c r="I173" s="2" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="174" spans="1:9">
@@ -6188,7 +6185,7 @@
         <v>329</v>
       </c>
       <c r="I174" s="2" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="175" spans="1:9">
@@ -6205,7 +6202,7 @@
         <v>308</v>
       </c>
       <c r="I175" s="2" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="176" spans="1:9">
@@ -6222,7 +6219,7 @@
         <v>307</v>
       </c>
       <c r="I176" s="2" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="177" spans="1:9">
@@ -6239,7 +6236,7 @@
         <v>330</v>
       </c>
       <c r="I177" s="2" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="178" spans="1:9">
@@ -6256,7 +6253,7 @@
         <v>311</v>
       </c>
       <c r="I178" s="2" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="179" spans="1:9">
@@ -6273,7 +6270,7 @@
         <v>331</v>
       </c>
       <c r="I179" s="2" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="180" spans="1:9">
@@ -6290,7 +6287,7 @@
         <v>331</v>
       </c>
       <c r="I180" s="2" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="181" spans="1:9">
@@ -6307,7 +6304,7 @@
         <v>332</v>
       </c>
       <c r="I181" s="2" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="182" spans="1:9">
@@ -6324,7 +6321,7 @@
         <v>333</v>
       </c>
       <c r="I182" s="2" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="183" spans="1:9">
@@ -6341,7 +6338,7 @@
         <v>308</v>
       </c>
       <c r="I183" s="2" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="184" spans="1:9">
@@ -6358,7 +6355,7 @@
         <v>308</v>
       </c>
       <c r="I184" s="2" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="185" spans="1:9">
@@ -6375,7 +6372,7 @@
         <v>307</v>
       </c>
       <c r="I185" s="2" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="186" spans="1:9">
@@ -6392,7 +6389,7 @@
         <v>308</v>
       </c>
       <c r="I186" s="2" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="187" spans="1:9">
@@ -6409,7 +6406,7 @@
         <v>308</v>
       </c>
       <c r="I187" s="2" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="188" spans="1:9">
@@ -6426,7 +6423,7 @@
         <v>308</v>
       </c>
       <c r="I188" s="2" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="189" spans="1:9">
@@ -6443,7 +6440,7 @@
         <v>1</v>
       </c>
       <c r="E189" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="190" spans="1:9">
@@ -6460,7 +6457,7 @@
         <v>334</v>
       </c>
       <c r="I190" s="2" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="191" spans="1:9">
@@ -6477,7 +6474,7 @@
         <v>312</v>
       </c>
       <c r="I191" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="192" spans="1:9">
@@ -6494,7 +6491,7 @@
         <v>335</v>
       </c>
       <c r="I192" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="193" spans="1:9">
@@ -6511,7 +6508,7 @@
         <v>314</v>
       </c>
       <c r="I193" s="2" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="194" spans="1:9">
@@ -6528,7 +6525,7 @@
         <v>311</v>
       </c>
       <c r="I194" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="195" spans="1:9">
@@ -6545,7 +6542,7 @@
         <v>307</v>
       </c>
       <c r="I195" s="2" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="196" spans="1:9">
@@ -6562,7 +6559,7 @@
         <v>336</v>
       </c>
       <c r="I196" s="2" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="197" spans="1:9">
@@ -6579,7 +6576,7 @@
         <v>312</v>
       </c>
       <c r="I197" s="2" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="198" spans="1:9">
@@ -6596,7 +6593,7 @@
         <v>335</v>
       </c>
       <c r="I198" s="2" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="199" spans="1:9">
@@ -6613,7 +6610,7 @@
         <v>314</v>
       </c>
       <c r="I199" s="2" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="200" spans="1:9">
@@ -6658,7 +6655,7 @@
         <v>1</v>
       </c>
       <c r="E202" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="203" spans="1:9">
@@ -6686,7 +6683,7 @@
         <v>276</v>
       </c>
       <c r="D204" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
     </row>
     <row r="205" spans="1:9">
@@ -6700,7 +6697,7 @@
         <v>276</v>
       </c>
       <c r="D205" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="206" spans="1:9">
@@ -6728,7 +6725,7 @@
         <v>277</v>
       </c>
       <c r="D207" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="208" spans="1:9">
@@ -6742,7 +6739,7 @@
         <v>276</v>
       </c>
       <c r="D208" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="209" spans="1:5">
@@ -6756,7 +6753,7 @@
         <v>278</v>
       </c>
       <c r="D209" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="210" spans="1:5">
@@ -6770,7 +6767,7 @@
         <v>5</v>
       </c>
       <c r="D210" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="211" spans="1:5">
@@ -6784,10 +6781,10 @@
         <v>5</v>
       </c>
       <c r="D211" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E211" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="212" spans="1:5">
@@ -6801,7 +6798,7 @@
         <v>279</v>
       </c>
       <c r="D212" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="213" spans="1:5">
@@ -6815,7 +6812,7 @@
         <v>280</v>
       </c>
       <c r="D213" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="214" spans="1:5">
@@ -6829,10 +6826,10 @@
         <v>5</v>
       </c>
       <c r="D214" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E214" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="215" spans="1:5">
@@ -6846,7 +6843,7 @@
         <v>281</v>
       </c>
       <c r="D215" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="216" spans="1:5">
@@ -6860,7 +6857,7 @@
         <v>282</v>
       </c>
       <c r="D216" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="217" spans="1:5">
@@ -6874,7 +6871,7 @@
         <v>282</v>
       </c>
       <c r="D217" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="218" spans="1:5">
@@ -6888,7 +6885,7 @@
         <v>282</v>
       </c>
       <c r="D218" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="219" spans="1:5">
@@ -6902,7 +6899,7 @@
         <v>282</v>
       </c>
       <c r="D219" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
   </sheetData>
@@ -7059,37 +7056,36 @@
     <hyperlink ref="I166" r:id="rId150"/>
     <hyperlink ref="I167" r:id="rId151"/>
     <hyperlink ref="I168" r:id="rId152"/>
-    <hyperlink ref="D169" r:id="rId153"/>
-    <hyperlink ref="I169" r:id="rId154"/>
-    <hyperlink ref="I170" r:id="rId155"/>
-    <hyperlink ref="I171" r:id="rId156"/>
-    <hyperlink ref="I172" r:id="rId157"/>
-    <hyperlink ref="I173" r:id="rId158"/>
-    <hyperlink ref="I174" r:id="rId159"/>
-    <hyperlink ref="I175" r:id="rId160"/>
-    <hyperlink ref="I176" r:id="rId161"/>
-    <hyperlink ref="I177" r:id="rId162"/>
-    <hyperlink ref="I178" r:id="rId163"/>
-    <hyperlink ref="I179" r:id="rId164"/>
-    <hyperlink ref="I180" r:id="rId165"/>
-    <hyperlink ref="I181" r:id="rId166"/>
-    <hyperlink ref="I182" r:id="rId167"/>
-    <hyperlink ref="I183" r:id="rId168"/>
-    <hyperlink ref="I184" r:id="rId169"/>
-    <hyperlink ref="I185" r:id="rId170"/>
-    <hyperlink ref="I186" r:id="rId171"/>
-    <hyperlink ref="I187" r:id="rId172"/>
-    <hyperlink ref="I188" r:id="rId173"/>
-    <hyperlink ref="I190" r:id="rId174"/>
-    <hyperlink ref="I191" r:id="rId175"/>
-    <hyperlink ref="I192" r:id="rId176"/>
-    <hyperlink ref="I193" r:id="rId177"/>
-    <hyperlink ref="I194" r:id="rId178"/>
-    <hyperlink ref="I195" r:id="rId179"/>
-    <hyperlink ref="I196" r:id="rId180"/>
-    <hyperlink ref="I197" r:id="rId181"/>
-    <hyperlink ref="I198" r:id="rId182"/>
-    <hyperlink ref="I199" r:id="rId183"/>
+    <hyperlink ref="I169" r:id="rId153"/>
+    <hyperlink ref="I170" r:id="rId154"/>
+    <hyperlink ref="I171" r:id="rId155"/>
+    <hyperlink ref="I172" r:id="rId156"/>
+    <hyperlink ref="I173" r:id="rId157"/>
+    <hyperlink ref="I174" r:id="rId158"/>
+    <hyperlink ref="I175" r:id="rId159"/>
+    <hyperlink ref="I176" r:id="rId160"/>
+    <hyperlink ref="I177" r:id="rId161"/>
+    <hyperlink ref="I178" r:id="rId162"/>
+    <hyperlink ref="I179" r:id="rId163"/>
+    <hyperlink ref="I180" r:id="rId164"/>
+    <hyperlink ref="I181" r:id="rId165"/>
+    <hyperlink ref="I182" r:id="rId166"/>
+    <hyperlink ref="I183" r:id="rId167"/>
+    <hyperlink ref="I184" r:id="rId168"/>
+    <hyperlink ref="I185" r:id="rId169"/>
+    <hyperlink ref="I186" r:id="rId170"/>
+    <hyperlink ref="I187" r:id="rId171"/>
+    <hyperlink ref="I188" r:id="rId172"/>
+    <hyperlink ref="I190" r:id="rId173"/>
+    <hyperlink ref="I191" r:id="rId174"/>
+    <hyperlink ref="I192" r:id="rId175"/>
+    <hyperlink ref="I193" r:id="rId176"/>
+    <hyperlink ref="I194" r:id="rId177"/>
+    <hyperlink ref="I195" r:id="rId178"/>
+    <hyperlink ref="I196" r:id="rId179"/>
+    <hyperlink ref="I197" r:id="rId180"/>
+    <hyperlink ref="I198" r:id="rId181"/>
+    <hyperlink ref="I199" r:id="rId182"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>